<commit_message>
Fixed search_step in read_branch
</commit_message>
<xml_diff>
--- a/send_email/attachments/5829786533/send.xlsx
+++ b/send_email/attachments/5829786533/send.xlsx
@@ -14,93 +14,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="38">
-  <si>
-    <t>2022-03-21</t>
-  </si>
-  <si>
-    <t>2022-02-15</t>
-  </si>
-  <si>
-    <t>2022-01-05</t>
-  </si>
-  <si>
-    <t>2022-01-15</t>
-  </si>
-  <si>
-    <t>2022-01-20</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>542/2-5</t>
-  </si>
-  <si>
-    <t>539\1-5</t>
-  </si>
-  <si>
-    <t>539/1-5</t>
-  </si>
-  <si>
-    <t>Замечание от цеха по поводу размера штока тормозной камеры на чертеже подвески - не указана длина</t>
-  </si>
-  <si>
-    <t>Почти на всех рамах отверстия для установки противооткатов перекрывается боковым лонжероном</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Привезли тумблер стробоскопов другого образца, неподходящий под кронштейн      </t>
-  </si>
-  <si>
-    <t>Привезли систему оптилинк вместо смарт-борда</t>
-  </si>
-  <si>
-    <t>Г образный разъемы для задних фонарей упираются в кронштейны для задних опор. Причина заключается в том что задние фонари пришли не по КД.</t>
-  </si>
-  <si>
-    <t>Фонари в комплектах электрооборудования пришли не по КД, заместо W137DL/W137DP пришли А.3776.005П-01, из за этого получился вредный контакт с направляющей трапа.</t>
-  </si>
-  <si>
-    <t>Неправильно подключили к модулятору блок управления OptiLink</t>
-  </si>
-  <si>
-    <t>СЗ№03/0129</t>
-  </si>
-  <si>
-    <t>Без СЗ</t>
-  </si>
-  <si>
-    <t>без СЗ, пересверлили крышку тумблера, чтобы подходил под кронштейн</t>
-  </si>
-  <si>
-    <t>СЗ№03/0002</t>
-  </si>
-  <si>
-    <t>Без СЗ. Срезали лишнее</t>
-  </si>
-  <si>
-    <t>Без СЗ. Установили с вредным контактом.</t>
-  </si>
-  <si>
-    <t>Без СЗ. Подключили правильно.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
+  <si>
+    <t>2023-02-27</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>ЫЫЫЫЫЫЫЫЫЫЫЫЫЫ</t>
+  </si>
+  <si>
+    <t>ЫЫЫЫЫЫЫЫЫЫЫЫЫЫЫЫ</t>
+  </si>
+  <si>
+    <t>ЫЫЫЫЫЫЫЫЫЫЫЫЫЫЫЫЫЫЫЫ</t>
+  </si>
+  <si>
+    <t>rtr</t>
   </si>
   <si>
     <t>Проблема решена</t>
   </si>
   <si>
-    <t>99064хх-0000100-01</t>
-  </si>
-  <si>
-    <t>Производство</t>
-  </si>
-  <si>
-    <t>Снабжение</t>
+    <t>КЕКхххх-0000КЕК-КЕК</t>
   </si>
   <si>
     <t>Шелепов</t>
-  </si>
-  <si>
-    <t>Гибадуллин</t>
   </si>
   <si>
     <t>Номер в базе данных</t>
@@ -501,7 +441,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:J8"/>
+  <dimension ref="B1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -517,231 +457,117 @@
   <sheetData>
     <row r="1" spans="2:10">
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="2" spans="2:10" s="2" customFormat="1" ht="82.45" customHeight="1">
+    <row r="2" spans="2:10" s="2" customFormat="1" ht="20" customHeight="1">
       <c r="B2" s="2">
-        <v>48</v>
+        <v>201</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" s="2" customFormat="1" ht="13.6" customHeight="1">
+      <c r="B3" s="2">
+        <v>202</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" s="2" customFormat="1" ht="17" customHeight="1">
+      <c r="B4" s="2">
+        <v>203</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" s="2" customFormat="1" ht="20" customHeight="1">
+      <c r="B5" s="2">
+        <v>204</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" s="2" customFormat="1" ht="77.35" customHeight="1">
-      <c r="B3" s="2">
-        <v>112</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" s="2" customFormat="1" ht="67.15" customHeight="1">
-      <c r="B4" s="2">
-        <v>144</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" s="2" customFormat="1" ht="37.4" customHeight="1">
-      <c r="B5" s="2">
-        <v>145</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="J5" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" s="2" customFormat="1" ht="117.3" customHeight="1">
-      <c r="B6" s="2">
-        <v>146</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" s="2" customFormat="1" ht="136.85" customHeight="1">
-      <c r="B7" s="2">
-        <v>147</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" s="2" customFormat="1" ht="51" customHeight="1">
-      <c r="B8" s="2">
-        <v>148</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added order by date in read branch sql queries
</commit_message>
<xml_diff>
--- a/send_email/attachments/5829786533/send.xlsx
+++ b/send_email/attachments/5829786533/send.xlsx
@@ -14,33 +14,144 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
-  <si>
-    <t>2023-02-27</t>
-  </si>
-  <si>
-    <t>123</t>
-  </si>
-  <si>
-    <t>ЫЫЫЫЫЫЫЫЫЫЫЫЫЫ</t>
-  </si>
-  <si>
-    <t>ЫЫЫЫЫЫЫЫЫЫЫЫЫЫЫЫ</t>
-  </si>
-  <si>
-    <t>ЫЫЫЫЫЫЫЫЫЫЫЫЫЫЫЫЫЫЫЫ</t>
-  </si>
-  <si>
-    <t>rtr</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="55">
+  <si>
+    <t>2021-03-24</t>
+  </si>
+  <si>
+    <t>2022-02-28</t>
+  </si>
+  <si>
+    <t>2022-03-16</t>
+  </si>
+  <si>
+    <t>2022-03-17</t>
+  </si>
+  <si>
+    <t>2022-03-19</t>
+  </si>
+  <si>
+    <t>2022-03-24</t>
+  </si>
+  <si>
+    <t>2022-03-25</t>
+  </si>
+  <si>
+    <t>2022-03-26</t>
+  </si>
+  <si>
+    <t>022/1-4</t>
+  </si>
+  <si>
+    <t>Скобы в установке прутков мешают дальнешйему монтажу жгутов электрики и пневматики на хомуты.</t>
+  </si>
+  <si>
+    <t>Оттяжная пружина из монтажа пневмопривода не имеет возможности крепления</t>
+  </si>
+  <si>
+    <t>Нет возможности установить задние последние боковые фонари - нет кронштейна</t>
+  </si>
+  <si>
+    <t>Накладка лонжерона перекрывает отверстие предназнченное для монтажа кронштейнов подставок</t>
+  </si>
+  <si>
+    <t>Ошибка в КД - не предусмотено крепление пневмопривода и жгутов электрики</t>
+  </si>
+  <si>
+    <t>Ошибка в КД - заложено неправильное количество кронштейнов 9911-2801508-10-В и 9911-2801508-В</t>
+  </si>
+  <si>
+    <t>Деталь 9911-2801442-В, изготовлена из 2-х частей, в чертеже не указано что возможно изготовлять из 2-х частей, в техпроцессе ПЗЦ идут 2 части, возможности изготовления цельной детали производству нет возможности, нужно КО-1 прописать в тех условиях о том что допускается изготовлять из 2-х частей. ВП не принимает такое</t>
+  </si>
+  <si>
+    <t xml:space="preserve">деталь 9911-2801442-В, не выдержан габаритный размер 120мм. Отклонение до 7мм. Ось 9911-2801452-В не полностью прилегает на отверстие кронштейна. </t>
+  </si>
+  <si>
+    <t>В раме 9911-2801010-В, в альбомном чертеже нет кронштейна указателя угла наклона, в чертеже в архиве ОГК он имеется, чертежи различаются</t>
+  </si>
+  <si>
+    <t>При установке кронштейнов подвески 9911-2900003-В не установили кронштейны 603113-2918058 и 603113-2918059 на ССЦ</t>
+  </si>
+  <si>
+    <t>Размер 250 до кронштейна ускорительного клапана в установке 9911-3500008-В недостаточен, вероятность вредного контакта с полкой лонжерона полиамидной трубки.</t>
+  </si>
+  <si>
+    <t>Не установили кронштейны блоков 305000-3508120 из установки кронштейнов стояночного тормоза 9911-3508003-В на ССЦ.</t>
+  </si>
+  <si>
+    <t>На правой полке лонжерона в средней группе отверстий, предназначенной для установки отбойника, нет резьбы.</t>
+  </si>
+  <si>
+    <t>Левая нижняя полка лонжерона изготовлена из частей, как следствие часть полки с отверстиями соориентирована не верно - развернута на 180 градусов.</t>
+  </si>
+  <si>
+    <t>Приварены кронштейны крыльев согласно графике чертежа, хотя никаких дополнительных указаний в виде технических требований или размеров в чертеже нет.</t>
+  </si>
+  <si>
+    <t>Жгуты электрики имеют недостаточную длину по боковым фонарям</t>
+  </si>
+  <si>
+    <t>По чертежу Э/О на левый боковой фонарь гусачной части жгут идет по стенке лонжерона, но в поперечине возле опорного устройства нет отверстий чтобы пропустить жгут, тянуть через правый борт не получится из-за длины проводки</t>
+  </si>
+  <si>
+    <t>Сразеали скобы</t>
+  </si>
+  <si>
+    <t>Без СЗ</t>
+  </si>
+  <si>
+    <t>Извещение от КО-1</t>
+  </si>
+  <si>
+    <t>Осталось лишних 32 кронштейна</t>
+  </si>
+  <si>
+    <t>Доработка согласно разрешению на отклонение от КО-1</t>
+  </si>
+  <si>
+    <t>Нет</t>
+  </si>
+  <si>
+    <t>Доварили на сборке</t>
+  </si>
+  <si>
+    <t>Применили угловые штуцеры по СЗ от КО-1</t>
+  </si>
+  <si>
+    <t>Нарезали резьбу</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Пересверливали отверстия </t>
+  </si>
+  <si>
+    <t>Срезали кронштейны крыльев</t>
+  </si>
+  <si>
+    <t>Доработка жгутов электрики по СЗ от КО-1</t>
+  </si>
+  <si>
+    <t>СЗ №03/137</t>
+  </si>
+  <si>
+    <t>Требует решения</t>
   </si>
   <si>
     <t>Проблема решена</t>
   </si>
   <si>
-    <t>КЕКхххх-0000КЕК-КЕК</t>
+    <t>9911ххх-0000063</t>
+  </si>
+  <si>
+    <t>КО</t>
+  </si>
+  <si>
+    <t>Производство</t>
   </si>
   <si>
     <t>Шелепов</t>
+  </si>
+  <si>
+    <t>Гибадуллин</t>
   </si>
   <si>
     <t>Номер в базе данных</t>
@@ -441,7 +552,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:J5"/>
+  <dimension ref="B1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -457,117 +568,524 @@
   <sheetData>
     <row r="1" spans="2:10">
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="2:10" s="2" customFormat="1" ht="20" customHeight="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" s="2" customFormat="1" ht="83.7" customHeight="1">
       <c r="B2" s="2">
-        <v>201</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" s="2" customFormat="1" ht="64.8" customHeight="1">
+      <c r="B3" s="2">
+        <v>30</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" s="2" customFormat="1" ht="67.5" customHeight="1">
+      <c r="B4" s="2">
+        <v>31</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" s="2" customFormat="1" ht="80.1" customHeight="1">
+      <c r="B5" s="2">
+        <v>32</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" s="2" customFormat="1" ht="64.8" customHeight="1">
+      <c r="B6" s="2">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" s="2" customFormat="1" ht="83.7" customHeight="1">
+      <c r="B7" s="2">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" s="2" customFormat="1" ht="287.1" customHeight="1">
+      <c r="B8" s="2">
+        <v>18</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" s="2" customFormat="1" ht="131.4" customHeight="1">
+      <c r="B9" s="2">
+        <v>19</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" s="2" customFormat="1" ht="122.4" customHeight="1">
+      <c r="B10" s="2">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" s="2" customFormat="1" ht="101.7" customHeight="1">
+      <c r="B11" s="2">
+        <v>21</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" s="2" customFormat="1" ht="141.3" customHeight="1">
+      <c r="B12" s="2">
+        <v>22</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" s="2" customFormat="1" ht="102.6" customHeight="1">
+      <c r="B13" s="2">
+        <v>23</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" s="2" customFormat="1" ht="95.4" customHeight="1">
+      <c r="B14" s="2">
+        <v>24</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" s="2" customFormat="1" ht="131.4" customHeight="1">
+      <c r="B15" s="2">
+        <v>25</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" s="2" customFormat="1" ht="134.1" customHeight="1">
+      <c r="B16" s="2">
+        <v>27</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" s="2" customFormat="1" ht="54" customHeight="1">
+      <c r="B17" s="2">
+        <v>28</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="D17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" s="2" customFormat="1" ht="199.8" customHeight="1">
+      <c r="B18" s="2">
+        <v>29</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" s="2" customFormat="1" ht="13.6" customHeight="1">
-      <c r="B3" s="2">
-        <v>202</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" s="2" customFormat="1" ht="17" customHeight="1">
-      <c r="B4" s="2">
-        <v>203</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" s="2" customFormat="1" ht="20" customHeight="1">
-      <c r="B5" s="2">
-        <v>204</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>8</v>
+      <c r="D18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>